<commit_message>
OWS - sprawko #3. Połowa roboty za nami
</commit_message>
<xml_diff>
--- a/OWS/Zadanie03/Testy/tabelki.xlsx
+++ b/OWS/Zadanie03/Testy/tabelki.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="Sito Domenowe" sheetId="1" r:id="rId1"/>
     <sheet name="Sito Funkcyjne" sheetId="2" r:id="rId2"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="Dzielenie" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="62">
   <si>
     <t>Czas pracy procesorów</t>
   </si>
@@ -181,6 +181,27 @@
   </si>
   <si>
     <t>Względny procentowy koszt zrównoleglenia</t>
+  </si>
+  <si>
+    <t>Dzielenie &lt;2, 60000000&gt;</t>
+  </si>
+  <si>
+    <t>Static 2P</t>
+  </si>
+  <si>
+    <t>Dynamic 2P</t>
+  </si>
+  <si>
+    <t>Static 4P</t>
+  </si>
+  <si>
+    <t>Dynamic 4P</t>
+  </si>
+  <si>
+    <t>Dzielenie &lt;2, 30000000&gt;</t>
+  </si>
+  <si>
+    <t>Dzielenie &lt;30000000, 60000000&gt;</t>
   </si>
 </sst>
 </file>
@@ -516,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M142"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O139" sqref="O139"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5164,8 +5185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="O140" sqref="O140"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8447,7 +8468,7 @@
         <v>0.9824312443654919</v>
       </c>
       <c r="D103">
-        <f t="shared" ref="D103:N103" si="41">D102/2</f>
+        <f t="shared" ref="D103:M103" si="41">D102/2</f>
         <v>0.74701331610027277</v>
       </c>
       <c r="E103">
@@ -9810,12 +9831,564 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>53.514964999999997</v>
+      </c>
+      <c r="C4">
+        <v>53.394907000000003</v>
+      </c>
+      <c r="D4">
+        <v>53.254134000000001</v>
+      </c>
+      <c r="E4">
+        <v>54.222887999999998</v>
+      </c>
+      <c r="F4">
+        <v>56.061537000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>53.541094000000001</v>
+      </c>
+      <c r="C5">
+        <v>33.544882999999999</v>
+      </c>
+      <c r="D5">
+        <v>26.628034</v>
+      </c>
+      <c r="E5">
+        <v>18.165392000000001</v>
+      </c>
+      <c r="F5">
+        <v>14.045322000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <f>$B5/C5</f>
+        <v>1.5961031672103314</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:F6" si="0">$B5/D5</f>
+        <v>2.0107039821265063</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>2.9474229898259283</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>3.8120232487371952</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7">
+        <f>C6/2</f>
+        <v>0.7980515836051657</v>
+      </c>
+      <c r="D7">
+        <f>D6/2</f>
+        <v>1.0053519910632531</v>
+      </c>
+      <c r="E7">
+        <f>E6/4</f>
+        <v>0.73685574745648208</v>
+      </c>
+      <c r="F7">
+        <f>F6/4</f>
+        <v>0.95300581218429881</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <f>59999999/B5</f>
+        <v>1120634.5354093811</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:F8" si="1">59999999/C5</f>
+        <v>1788648.3312521914</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>2253264.3228561296</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>3302983.9928585081</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>4271884.9023183659</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9">
+        <f>(C10/C5)*100</f>
+        <v>40.825478508898044</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:F9" si="2">(D10/D5)*100</f>
+        <v>7.2630221217178407E-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>101.50444317414127</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>0.85260416243928638</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10">
+        <f>(2*C5)-C4</f>
+        <v>13.694858999999994</v>
+      </c>
+      <c r="D10">
+        <f>(2*D5)-D4</f>
+        <v>1.933999999998548E-3</v>
+      </c>
+      <c r="E10">
+        <f>(4*E5)-E4</f>
+        <v>18.438680000000005</v>
+      </c>
+      <c r="F10">
+        <f>(4*F5)-F4</f>
+        <v>0.11975100000000083</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>19.453053000000001</v>
+      </c>
+      <c r="C16">
+        <v>19.526676999999999</v>
+      </c>
+      <c r="D16">
+        <v>20.011507999999999</v>
+      </c>
+      <c r="E16">
+        <v>20.218921999999999</v>
+      </c>
+      <c r="F16">
+        <v>21.075406999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>19.453543</v>
+      </c>
+      <c r="C17">
+        <v>12.218143</v>
+      </c>
+      <c r="D17">
+        <v>10.007332999999999</v>
+      </c>
+      <c r="E17">
+        <v>6.7555699999999996</v>
+      </c>
+      <c r="F17">
+        <v>5.2832530000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18">
+        <f>$B17/C17</f>
+        <v>1.5921849171351163</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:F18" si="3">$B17/D17</f>
+        <v>1.9439288169984952</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>2.8796301422381827</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>3.6821145987140875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <f>C18/2</f>
+        <v>0.79609245856755817</v>
+      </c>
+      <c r="D19">
+        <f>D18/2</f>
+        <v>0.97196440849924759</v>
+      </c>
+      <c r="E19">
+        <f>E18/4</f>
+        <v>0.71990753555954567</v>
+      </c>
+      <c r="F19">
+        <f>F18/4</f>
+        <v>0.92052864967852188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <f>29999999/B17</f>
+        <v>1542135.4865794885</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:F20" si="4">29999999/C17</f>
+        <v>2455364.861910685</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="4"/>
+        <v>2997801.6120778634</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
+        <v>4440779.8305694414</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="4"/>
+        <v>5678319.5883293869</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21">
+        <f>(C22/C17)*100</f>
+        <v>40.182939420499494</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:F21" si="5">(D22/D17)*100</f>
+        <v>3.1556859355026022E-2</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="5"/>
+        <v>100.70738664539039</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>1.0903320359634934</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22">
+        <f>(2*C17)-C16</f>
+        <v>4.9096089999999997</v>
+      </c>
+      <c r="D22">
+        <f>(2*D17)-D16</f>
+        <v>3.157999999999106E-3</v>
+      </c>
+      <c r="E22">
+        <f>(4*E17)-E16</f>
+        <v>6.8033579999999994</v>
+      </c>
+      <c r="F22">
+        <f>(4*F17)-F16</f>
+        <v>5.7605000000002349E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>33.452007000000002</v>
+      </c>
+      <c r="C28">
+        <v>32.94529</v>
+      </c>
+      <c r="D28">
+        <v>33.304583000000001</v>
+      </c>
+      <c r="E28">
+        <v>34.353786999999997</v>
+      </c>
+      <c r="F28">
+        <v>34.977938999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>33.453254000000001</v>
+      </c>
+      <c r="C29">
+        <v>17.648728999999999</v>
+      </c>
+      <c r="D29">
+        <v>16.653236</v>
+      </c>
+      <c r="E29">
+        <v>9.47133</v>
+      </c>
+      <c r="F29">
+        <v>8.7621710000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30">
+        <f>$B29/C29</f>
+        <v>1.895504996422122</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30:F30" si="6">$B29/D29</f>
+        <v>2.0088140226920461</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="6"/>
+        <v>3.5320545266609864</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="6"/>
+        <v>3.8179184131421309</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31">
+        <f>C30/2</f>
+        <v>0.947752498211061</v>
+      </c>
+      <c r="D31">
+        <f>D30/2</f>
+        <v>1.0044070113460231</v>
+      </c>
+      <c r="E31">
+        <f>E30/4</f>
+        <v>0.8830136316652466</v>
+      </c>
+      <c r="F31">
+        <f>F30/4</f>
+        <v>0.95447960328553272</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32">
+        <f>30000001/B29</f>
+        <v>896773.77871820773</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:F32" si="7">30000001/C29</f>
+        <v>1699839.1782207093</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="7"/>
+        <v>1801451.7418716699</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="7"/>
+        <v>3167453.8845125237</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="7"/>
+        <v>3423809.1221912922</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33">
+        <f>(C34/C29)*100</f>
+        <v>13.327690622933805</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ref="D33:F33" si="8">(D34/D29)*100</f>
+        <v>1.1343140756538099E-2</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="8"/>
+        <v>37.286558487561969</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="8"/>
+        <v>0.80739122758506177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34">
+        <f>(2*C29)-C28</f>
+        <v>2.3521679999999989</v>
+      </c>
+      <c r="D34">
+        <f>(2*D29)-D28</f>
+        <v>1.8889999999984752E-3</v>
+      </c>
+      <c r="E34">
+        <f>(4*E29)-E28</f>
+        <v>3.5315330000000031</v>
+      </c>
+      <c r="F34">
+        <f>(4*F29)-F28</f>
+        <v>7.0745000000002278E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>